<commit_message>
consolida XLSX de carpeta "grupos"
</commit_message>
<xml_diff>
--- a/Datos/libros/convert/xlsx/Anónimo - Lazarillo de Tormes_esp.xlsx
+++ b/Datos/libros/convert/xlsx/Anónimo - Lazarillo de Tormes_esp.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f7ba5ab37b782061/Estudios/UNI/Curso NLP/Proyecto/Traductor-Quechua-Spanish-Spanish-Quechua/Datos/libros/convert/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f7ba5ab37b782061/Estudios/UNI/Curso NLP/Proyecto/Traductor-Quechua-Spanish-Spanish-Quechua/Datos/libros/convert/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BE28E0DD-9BA0-4D33-968B-ECD6F925A22E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="8_{BE28E0DD-9BA0-4D33-968B-ECD6F925A22E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D7759097-CAE8-456B-8D52-EFE39ED1B8E8}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="0" windowWidth="28800" windowHeight="31800" xr2:uid="{23D5DA03-EFC5-41FA-8A6B-AB2356089BE4}"/>
+    <workbookView xWindow="5460" yWindow="5460" windowWidth="43200" windowHeight="23535" xr2:uid="{23D5DA03-EFC5-41FA-8A6B-AB2356089BE4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2586,9 +2586,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2905,239 +2903,242 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F053A83-9E84-499C-B5EA-9D1D3E0652BB}">
   <dimension ref="A1:A780"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="A759" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="A789" sqref="A789"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="120.28515625" style="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="A34" s="1" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="A35" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="A36" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="A37" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="A38" s="1" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="A39" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="A40" s="1" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="A41" s="1" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="A42" s="1" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="A43" s="1" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="A44" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="A45" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="A46" s="1" t="s">
         <v>45</v>
       </c>
     </row>
@@ -3147,188 +3148,188 @@
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="A48" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+      <c r="A49" s="1" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+      <c r="A50" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+      <c r="A51" s="1" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+      <c r="A52" s="1" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+      <c r="A53" s="1" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+      <c r="A54" s="1" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+      <c r="A55" s="1" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+      <c r="A56" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+      <c r="A57" s="1" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+      <c r="A58" s="1" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+      <c r="A59" s="1" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+      <c r="A60" s="1" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+      <c r="A61" s="1" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+      <c r="A62" s="1" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+      <c r="A63" s="1" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+      <c r="A64" s="1" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+      <c r="A65" s="1" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+      <c r="A66" s="1" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+      <c r="A67" s="1" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+      <c r="A68" s="1" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+      <c r="A69" s="1" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+      <c r="A70" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+      <c r="A71" s="1" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+      <c r="A72" s="1" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
+      <c r="A73" s="1" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+      <c r="A74" s="1" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
+      <c r="A75" s="1" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
+      <c r="A76" s="1" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
+      <c r="A77" s="1" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
+      <c r="A78" s="1" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
+      <c r="A79" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A80" t="e">
+      <c r="A80" s="1" t="e">
         <f>-¿Qué diablo es esto, que después que conmigo estás no me dan sino  medias blancas, y de antes una blanca y un maravedí hartas veces me pagaban?</f>
         <v>#NAME?</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+      <c r="A81" s="1" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
+      <c r="A82" s="1" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
+      <c r="A83" s="1" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
+      <c r="A84" s="1" t="s">
         <v>82</v>
       </c>
     </row>
@@ -3338,67 +3339,67 @@
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
+      <c r="A86" s="1" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
+      <c r="A87" s="1" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
+      <c r="A88" s="1" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
+      <c r="A89" s="1" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
+      <c r="A90" s="1" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
+      <c r="A91" s="1" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
+      <c r="A92" s="1" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
+      <c r="A93" s="1" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
+      <c r="A94" s="1" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
+      <c r="A95" s="1" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
+      <c r="A96" s="1" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
+      <c r="A97" s="1" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
+      <c r="A98" s="1" t="s">
         <v>96</v>
       </c>
     </row>
@@ -3408,22 +3409,22 @@
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
+      <c r="A100" s="1" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
+      <c r="A101" s="1" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
+      <c r="A102" s="1" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
+      <c r="A103" s="1" t="s">
         <v>101</v>
       </c>
     </row>
@@ -3433,7 +3434,7 @@
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
+      <c r="A105" s="1" t="s">
         <v>103</v>
       </c>
     </row>
@@ -3443,87 +3444,87 @@
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
+      <c r="A107" s="1" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
+      <c r="A108" s="1" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
+      <c r="A109" s="1" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
+      <c r="A110" s="1" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
+      <c r="A111" s="1" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
+      <c r="A112" s="1" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
+      <c r="A113" s="1" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
+      <c r="A114" s="1" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
+      <c r="A115" s="1" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
+      <c r="A116" s="1" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
+      <c r="A117" s="1" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
+      <c r="A118" s="1" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
+      <c r="A119" s="1" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
+      <c r="A120" s="1" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
+      <c r="A121" s="1" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
+      <c r="A122" s="1" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
+      <c r="A123" s="1" t="s">
         <v>121</v>
       </c>
     </row>
@@ -3533,17 +3534,17 @@
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
+      <c r="A125" s="1" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
+      <c r="A126" s="1" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
+      <c r="A127" s="1" t="s">
         <v>125</v>
       </c>
     </row>
@@ -3553,12 +3554,12 @@
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
+      <c r="A129" s="1" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
+      <c r="A130" s="1" t="s">
         <v>128</v>
       </c>
     </row>
@@ -3568,47 +3569,47 @@
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
+      <c r="A132" s="1" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
+      <c r="A133" s="1" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
+      <c r="A134" s="1" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
+      <c r="A135" s="1" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
+      <c r="A136" s="1" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
+      <c r="A137" s="1" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
+      <c r="A138" s="1" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
+      <c r="A139" s="1" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
+      <c r="A140" s="1" t="s">
         <v>138</v>
       </c>
     </row>
@@ -3618,87 +3619,87 @@
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
+      <c r="A142" s="1" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
+      <c r="A143" s="1" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A144" t="s">
+      <c r="A144" s="1" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
+      <c r="A145" s="1" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
+      <c r="A146" s="1" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
+      <c r="A147" s="1" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
+      <c r="A148" s="1" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
+      <c r="A149" s="1" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A150" t="s">
+      <c r="A150" s="1" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
+      <c r="A151" s="1" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A152" t="s">
+      <c r="A152" s="1" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
+      <c r="A153" s="1" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A154" t="s">
+      <c r="A154" s="1" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A155" t="s">
+      <c r="A155" s="1" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A156" t="s">
+      <c r="A156" s="1" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A157" t="s">
+      <c r="A157" s="1" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A158" t="s">
+      <c r="A158" s="1" t="s">
         <v>156</v>
       </c>
     </row>
@@ -3708,87 +3709,87 @@
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A160" t="s">
+      <c r="A160" s="1" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A161" t="s">
+      <c r="A161" s="1" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A162" t="s">
+      <c r="A162" s="1" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A163" t="s">
+      <c r="A163" s="1" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A164" t="s">
+      <c r="A164" s="1" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A165" t="s">
+      <c r="A165" s="1" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A166" t="s">
+      <c r="A166" s="1" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A167" t="s">
+      <c r="A167" s="1" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A168" t="s">
+      <c r="A168" s="1" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A169" t="s">
+      <c r="A169" s="1" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A170" t="s">
+      <c r="A170" s="1" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A171" t="s">
+      <c r="A171" s="1" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A172" t="s">
+      <c r="A172" s="1" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A173" t="s">
+      <c r="A173" s="1" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A174" t="s">
+      <c r="A174" s="1" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A175" t="s">
+      <c r="A175" s="1" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A176" t="s">
+      <c r="A176" s="1" t="s">
         <v>174</v>
       </c>
     </row>
@@ -3798,7 +3799,7 @@
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A178" t="s">
+      <c r="A178" s="1" t="s">
         <v>176</v>
       </c>
     </row>
@@ -3808,32 +3809,32 @@
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A180" t="s">
+      <c r="A180" s="1" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A181" t="s">
+      <c r="A181" s="1" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A182" t="s">
+      <c r="A182" s="1" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A183" t="s">
+      <c r="A183" s="1" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A184" t="s">
+      <c r="A184" s="1" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A185" t="s">
+      <c r="A185" s="1" t="s">
         <v>183</v>
       </c>
     </row>
@@ -3843,22 +3844,22 @@
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A187" t="s">
+      <c r="A187" s="1" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A188" t="s">
+      <c r="A188" s="1" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A189" t="s">
+      <c r="A189" s="1" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A190" t="s">
+      <c r="A190" s="1" t="s">
         <v>188</v>
       </c>
     </row>
@@ -3868,27 +3869,27 @@
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A192" t="s">
+      <c r="A192" s="1" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A193" t="s">
+      <c r="A193" s="1" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A194" t="s">
+      <c r="A194" s="1" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A195" t="s">
+      <c r="A195" s="1" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A196" t="s">
+      <c r="A196" s="1" t="s">
         <v>194</v>
       </c>
     </row>
@@ -3898,7 +3899,7 @@
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A198" t="s">
+      <c r="A198" s="1" t="s">
         <v>196</v>
       </c>
     </row>
@@ -3908,52 +3909,52 @@
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A200" t="s">
+      <c r="A200" s="1" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A201" t="s">
+      <c r="A201" s="1" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A202" t="s">
+      <c r="A202" s="1" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A203" t="s">
+      <c r="A203" s="1" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A204" t="s">
+      <c r="A204" s="1" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A205" t="s">
+      <c r="A205" s="1" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A206" t="s">
+      <c r="A206" s="1" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A207" t="s">
+      <c r="A207" s="1" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A208" t="s">
+      <c r="A208" s="1" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A209" t="s">
+      <c r="A209" s="1" t="s">
         <v>207</v>
       </c>
     </row>
@@ -3963,157 +3964,157 @@
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A211" t="s">
+      <c r="A211" s="1" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A212" t="s">
+      <c r="A212" s="1" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A213" t="s">
+      <c r="A213" s="1" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A214" t="s">
+      <c r="A214" s="1" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A215" t="s">
+      <c r="A215" s="1" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="216" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A216" t="s">
+      <c r="A216" s="1" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="217" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A217" t="s">
+      <c r="A217" s="1" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="218" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A218" t="s">
+      <c r="A218" s="1" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A219" t="s">
+      <c r="A219" s="1" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="220" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A220" t="s">
+      <c r="A220" s="1" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="221" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A221" t="s">
+      <c r="A221" s="1" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="222" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A222" t="s">
+      <c r="A222" s="1" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="223" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A223" t="s">
+      <c r="A223" s="1" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="224" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A224" t="s">
+      <c r="A224" s="1" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="225" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A225" t="s">
+      <c r="A225" s="1" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="226" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A226" t="s">
+      <c r="A226" s="1" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="227" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A227" t="s">
+      <c r="A227" s="1" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="228" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A228" t="s">
+      <c r="A228" s="1" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="229" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A229" t="s">
+      <c r="A229" s="1" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="230" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A230" t="s">
+      <c r="A230" s="1" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="231" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A231" t="s">
+      <c r="A231" s="1" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="232" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A232" t="s">
+      <c r="A232" s="1" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="233" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A233" t="s">
+      <c r="A233" s="1" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="234" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A234" t="s">
+      <c r="A234" s="1" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="235" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A235" t="s">
+      <c r="A235" s="1" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="236" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A236" t="s">
+      <c r="A236" s="1" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="237" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A237" t="s">
+      <c r="A237" s="1" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="238" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A238" t="s">
+      <c r="A238" s="1" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="239" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A239" t="s">
+      <c r="A239" s="1" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="240" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A240" t="s">
+      <c r="A240" s="1" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="241" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A241" t="s">
+      <c r="A241" s="1" t="s">
         <v>239</v>
       </c>
     </row>
@@ -4123,77 +4124,77 @@
       </c>
     </row>
     <row r="243" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A243" t="s">
+      <c r="A243" s="1" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="244" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A244" t="s">
+      <c r="A244" s="1" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="245" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A245" t="s">
+      <c r="A245" s="1" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="246" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A246" t="s">
+      <c r="A246" s="1" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="247" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A247" t="s">
+      <c r="A247" s="1" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="248" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A248" t="s">
+      <c r="A248" s="1" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="249" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A249" t="s">
+      <c r="A249" s="1" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="250" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A250" t="s">
+      <c r="A250" s="1" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="251" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A251" t="s">
+      <c r="A251" s="1" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="252" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A252" t="s">
+      <c r="A252" s="1" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="253" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A253" t="s">
+      <c r="A253" s="1" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="254" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A254" t="s">
+      <c r="A254" s="1" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="255" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A255" t="s">
+      <c r="A255" s="1" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="256" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A256" t="s">
+      <c r="A256" s="1" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="257" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A257" t="s">
+      <c r="A257" s="1" t="s">
         <v>255</v>
       </c>
     </row>
@@ -4203,42 +4204,42 @@
       </c>
     </row>
     <row r="259" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A259" t="s">
+      <c r="A259" s="1" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="260" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A260" t="s">
+      <c r="A260" s="1" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="261" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A261" t="s">
+      <c r="A261" s="1" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="262" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A262" t="s">
+      <c r="A262" s="1" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="263" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A263" t="s">
+      <c r="A263" s="1" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="264" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A264" t="s">
+      <c r="A264" s="1" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="265" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A265" t="s">
+      <c r="A265" s="1" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="266" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A266" t="s">
+      <c r="A266" s="1" t="s">
         <v>264</v>
       </c>
     </row>
@@ -4248,27 +4249,27 @@
       </c>
     </row>
     <row r="268" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A268" t="s">
+      <c r="A268" s="1" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="269" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A269" t="s">
+      <c r="A269" s="1" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="270" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A270" t="s">
+      <c r="A270" s="1" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="271" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A271" t="s">
+      <c r="A271" s="1" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="272" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A272" t="s">
+      <c r="A272" s="1" t="s">
         <v>270</v>
       </c>
     </row>
@@ -4278,7 +4279,7 @@
       </c>
     </row>
     <row r="274" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A274" t="s">
+      <c r="A274" s="1" t="s">
         <v>272</v>
       </c>
     </row>
@@ -4288,32 +4289,32 @@
       </c>
     </row>
     <row r="276" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A276" t="s">
+      <c r="A276" s="1" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="277" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A277" t="s">
+      <c r="A277" s="1" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="278" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A278" t="s">
+      <c r="A278" s="1" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="279" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A279" t="s">
+      <c r="A279" s="1" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="280" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A280" t="s">
+      <c r="A280" s="1" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="281" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A281" t="s">
+      <c r="A281" s="1" t="s">
         <v>279</v>
       </c>
     </row>
@@ -4323,72 +4324,72 @@
       </c>
     </row>
     <row r="283" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A283" t="s">
+      <c r="A283" s="1" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="284" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A284" t="s">
+      <c r="A284" s="1" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="285" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A285" t="s">
+      <c r="A285" s="1" t="s">
         <v>283</v>
       </c>
     </row>
     <row r="286" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A286" t="s">
+      <c r="A286" s="1" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="287" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A287" t="s">
+      <c r="A287" s="1" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="288" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A288" t="s">
+      <c r="A288" s="1" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="289" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A289" t="s">
+      <c r="A289" s="1" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="290" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A290" t="s">
+      <c r="A290" s="1" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="291" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A291" t="s">
+      <c r="A291" s="1" t="s">
         <v>289</v>
       </c>
     </row>
     <row r="292" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A292" t="s">
+      <c r="A292" s="1" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="293" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A293" t="s">
+      <c r="A293" s="1" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="294" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A294" t="s">
+      <c r="A294" s="1" t="s">
         <v>292</v>
       </c>
     </row>
     <row r="295" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A295" t="s">
+      <c r="A295" s="1" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="296" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A296" t="s">
+      <c r="A296" s="1" t="s">
         <v>294</v>
       </c>
     </row>
@@ -4398,37 +4399,37 @@
       </c>
     </row>
     <row r="298" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A298" t="s">
+      <c r="A298" s="1" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="299" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A299" t="s">
+      <c r="A299" s="1" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="300" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A300" t="s">
+      <c r="A300" s="1" t="s">
         <v>298</v>
       </c>
     </row>
     <row r="301" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A301" t="s">
+      <c r="A301" s="1" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="302" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A302" t="s">
+      <c r="A302" s="1" t="s">
         <v>300</v>
       </c>
     </row>
     <row r="303" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A303" t="s">
+      <c r="A303" s="1" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="304" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A304" t="s">
+      <c r="A304" s="1" t="s">
         <v>302</v>
       </c>
     </row>
@@ -4438,27 +4439,27 @@
       </c>
     </row>
     <row r="306" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A306" t="s">
+      <c r="A306" s="1" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="307" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A307" t="s">
+      <c r="A307" s="1" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="308" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A308" t="s">
+      <c r="A308" s="1" t="s">
         <v>306</v>
       </c>
     </row>
     <row r="309" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A309" t="s">
+      <c r="A309" s="1" t="s">
         <v>307</v>
       </c>
     </row>
     <row r="310" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A310" t="s">
+      <c r="A310" s="1" t="s">
         <v>308</v>
       </c>
     </row>
@@ -4468,37 +4469,37 @@
       </c>
     </row>
     <row r="312" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A312" t="s">
+      <c r="A312" s="1" t="s">
         <v>310</v>
       </c>
     </row>
     <row r="313" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A313" t="s">
+      <c r="A313" s="1" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="314" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A314" t="s">
+      <c r="A314" s="1" t="s">
         <v>312</v>
       </c>
     </row>
     <row r="315" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A315" t="s">
+      <c r="A315" s="1" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="316" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A316" t="s">
+      <c r="A316" s="1" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="317" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A317" t="s">
+      <c r="A317" s="1" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="318" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A318" t="s">
+      <c r="A318" s="1" t="s">
         <v>316</v>
       </c>
     </row>
@@ -4508,192 +4509,192 @@
       </c>
     </row>
     <row r="320" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A320" t="s">
+      <c r="A320" s="1" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="321" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A321" t="s">
+      <c r="A321" s="1" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="322" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A322" t="s">
+      <c r="A322" s="1" t="s">
         <v>320</v>
       </c>
     </row>
     <row r="323" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A323" t="s">
+      <c r="A323" s="1" t="s">
         <v>321</v>
       </c>
     </row>
     <row r="324" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A324" t="s">
+      <c r="A324" s="1" t="s">
         <v>322</v>
       </c>
     </row>
     <row r="325" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A325" t="s">
+      <c r="A325" s="1" t="s">
         <v>323</v>
       </c>
     </row>
     <row r="326" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A326" t="s">
+      <c r="A326" s="1" t="s">
         <v>324</v>
       </c>
     </row>
     <row r="327" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A327" t="s">
+      <c r="A327" s="1" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="328" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A328" t="s">
+      <c r="A328" s="1" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="329" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A329" t="s">
+      <c r="A329" s="1" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="330" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A330" t="s">
+      <c r="A330" s="1" t="s">
         <v>328</v>
       </c>
     </row>
     <row r="331" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A331" t="s">
+      <c r="A331" s="1" t="s">
         <v>329</v>
       </c>
     </row>
     <row r="332" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A332" t="s">
+      <c r="A332" s="1" t="s">
         <v>330</v>
       </c>
     </row>
     <row r="333" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A333" t="s">
+      <c r="A333" s="1" t="s">
         <v>331</v>
       </c>
     </row>
     <row r="334" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A334" t="s">
+      <c r="A334" s="1" t="s">
         <v>332</v>
       </c>
     </row>
     <row r="335" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A335" t="s">
+      <c r="A335" s="1" t="s">
         <v>333</v>
       </c>
     </row>
     <row r="336" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A336" t="s">
+      <c r="A336" s="1" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="337" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A337" t="s">
+      <c r="A337" s="1" t="s">
         <v>335</v>
       </c>
     </row>
     <row r="338" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A338" t="s">
+      <c r="A338" s="1" t="s">
         <v>336</v>
       </c>
     </row>
     <row r="339" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A339" t="s">
+      <c r="A339" s="1" t="s">
         <v>337</v>
       </c>
     </row>
     <row r="340" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A340" t="s">
+      <c r="A340" s="1" t="s">
         <v>338</v>
       </c>
     </row>
     <row r="341" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A341" t="s">
+      <c r="A341" s="1" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="342" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A342" t="s">
+      <c r="A342" s="1" t="s">
         <v>340</v>
       </c>
     </row>
     <row r="343" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A343" t="s">
+      <c r="A343" s="1" t="s">
         <v>341</v>
       </c>
     </row>
     <row r="344" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A344" t="s">
+      <c r="A344" s="1" t="s">
         <v>342</v>
       </c>
     </row>
     <row r="345" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A345" t="s">
+      <c r="A345" s="1" t="s">
         <v>343</v>
       </c>
     </row>
     <row r="346" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A346" t="s">
+      <c r="A346" s="1" t="s">
         <v>344</v>
       </c>
     </row>
     <row r="347" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A347" t="s">
+      <c r="A347" s="1" t="s">
         <v>345</v>
       </c>
     </row>
     <row r="348" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A348" t="s">
+      <c r="A348" s="1" t="s">
         <v>346</v>
       </c>
     </row>
     <row r="349" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A349" t="s">
+      <c r="A349" s="1" t="s">
         <v>347</v>
       </c>
     </row>
     <row r="350" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A350" t="s">
+      <c r="A350" s="1" t="s">
         <v>348</v>
       </c>
     </row>
     <row r="351" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A351" t="s">
+      <c r="A351" s="1" t="s">
         <v>349</v>
       </c>
     </row>
     <row r="352" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A352" t="s">
+      <c r="A352" s="1" t="s">
         <v>350</v>
       </c>
     </row>
     <row r="353" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A353" t="s">
+      <c r="A353" s="1" t="s">
         <v>351</v>
       </c>
     </row>
     <row r="354" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A354" t="s">
+      <c r="A354" s="1" t="s">
         <v>352</v>
       </c>
     </row>
     <row r="355" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A355" t="s">
+      <c r="A355" s="1" t="s">
         <v>353</v>
       </c>
     </row>
     <row r="356" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A356" t="s">
+      <c r="A356" s="1" t="s">
         <v>354</v>
       </c>
     </row>
     <row r="357" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A357" t="s">
+      <c r="A357" s="1" t="s">
         <v>355</v>
       </c>
     </row>
@@ -4703,32 +4704,32 @@
       </c>
     </row>
     <row r="359" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A359" t="s">
+      <c r="A359" s="1" t="s">
         <v>357</v>
       </c>
     </row>
     <row r="360" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A360" t="s">
+      <c r="A360" s="1" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="361" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A361" t="s">
+      <c r="A361" s="1" t="s">
         <v>359</v>
       </c>
     </row>
     <row r="362" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A362" t="s">
+      <c r="A362" s="1" t="s">
         <v>360</v>
       </c>
     </row>
     <row r="363" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A363" t="s">
+      <c r="A363" s="1" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="364" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A364" t="s">
+      <c r="A364" s="1" t="s">
         <v>361</v>
       </c>
     </row>
@@ -4738,127 +4739,127 @@
       </c>
     </row>
     <row r="366" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A366" t="s">
+      <c r="A366" s="1" t="s">
         <v>363</v>
       </c>
     </row>
     <row r="367" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A367" t="s">
+      <c r="A367" s="1" t="s">
         <v>364</v>
       </c>
     </row>
     <row r="368" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A368" t="s">
+      <c r="A368" s="1" t="s">
         <v>365</v>
       </c>
     </row>
     <row r="369" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A369" t="s">
+      <c r="A369" s="1" t="s">
         <v>366</v>
       </c>
     </row>
     <row r="370" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A370" t="s">
+      <c r="A370" s="1" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="371" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A371" t="s">
+      <c r="A371" s="1" t="s">
         <v>368</v>
       </c>
     </row>
     <row r="372" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A372" t="s">
+      <c r="A372" s="1" t="s">
         <v>369</v>
       </c>
     </row>
     <row r="373" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A373" t="s">
+      <c r="A373" s="1" t="s">
         <v>370</v>
       </c>
     </row>
     <row r="374" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A374" t="s">
+      <c r="A374" s="1" t="s">
         <v>371</v>
       </c>
     </row>
     <row r="375" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A375" t="s">
+      <c r="A375" s="1" t="s">
         <v>372</v>
       </c>
     </row>
     <row r="376" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A376" t="s">
+      <c r="A376" s="1" t="s">
         <v>373</v>
       </c>
     </row>
     <row r="377" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A377" t="s">
+      <c r="A377" s="1" t="s">
         <v>374</v>
       </c>
     </row>
     <row r="378" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A378" t="s">
+      <c r="A378" s="1" t="s">
         <v>375</v>
       </c>
     </row>
     <row r="379" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A379" t="s">
+      <c r="A379" s="1" t="s">
         <v>376</v>
       </c>
     </row>
     <row r="380" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A380" t="s">
+      <c r="A380" s="1" t="s">
         <v>377</v>
       </c>
     </row>
     <row r="381" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A381" t="s">
+      <c r="A381" s="1" t="s">
         <v>378</v>
       </c>
     </row>
     <row r="382" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A382" t="s">
+      <c r="A382" s="1" t="s">
         <v>379</v>
       </c>
     </row>
     <row r="383" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A383" t="s">
+      <c r="A383" s="1" t="s">
         <v>380</v>
       </c>
     </row>
     <row r="384" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A384" t="s">
+      <c r="A384" s="1" t="s">
         <v>381</v>
       </c>
     </row>
     <row r="385" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A385" t="s">
+      <c r="A385" s="1" t="s">
         <v>382</v>
       </c>
     </row>
     <row r="386" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A386" t="s">
+      <c r="A386" s="1" t="s">
         <v>383</v>
       </c>
     </row>
     <row r="387" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A387" t="s">
+      <c r="A387" s="1" t="s">
         <v>384</v>
       </c>
     </row>
     <row r="388" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A388" t="s">
+      <c r="A388" s="1" t="s">
         <v>385</v>
       </c>
     </row>
     <row r="389" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A389" t="s">
+      <c r="A389" s="1" t="s">
         <v>386</v>
       </c>
     </row>
     <row r="390" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A390" t="s">
+      <c r="A390" s="1" t="s">
         <v>387</v>
       </c>
     </row>
@@ -4868,27 +4869,27 @@
       </c>
     </row>
     <row r="392" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A392" t="s">
+      <c r="A392" s="1" t="s">
         <v>389</v>
       </c>
     </row>
     <row r="393" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A393" t="s">
+      <c r="A393" s="1" t="s">
         <v>390</v>
       </c>
     </row>
     <row r="394" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A394" t="s">
+      <c r="A394" s="1" t="s">
         <v>391</v>
       </c>
     </row>
     <row r="395" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A395" t="s">
+      <c r="A395" s="1" t="s">
         <v>392</v>
       </c>
     </row>
     <row r="396" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A396" t="s">
+      <c r="A396" s="1" t="s">
         <v>393</v>
       </c>
     </row>
@@ -4908,12 +4909,12 @@
       </c>
     </row>
     <row r="400" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A400" t="s">
+      <c r="A400" s="1" t="s">
         <v>397</v>
       </c>
     </row>
     <row r="401" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A401" t="s">
+      <c r="A401" s="1" t="s">
         <v>398</v>
       </c>
     </row>
@@ -4923,17 +4924,17 @@
       </c>
     </row>
     <row r="403" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A403" t="s">
+      <c r="A403" s="1" t="s">
         <v>400</v>
       </c>
     </row>
     <row r="404" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A404" t="s">
+      <c r="A404" s="1" t="s">
         <v>401</v>
       </c>
     </row>
     <row r="405" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A405" t="s">
+      <c r="A405" s="1" t="s">
         <v>402</v>
       </c>
     </row>
@@ -4948,57 +4949,57 @@
       </c>
     </row>
     <row r="408" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A408" t="s">
+      <c r="A408" s="1" t="s">
         <v>405</v>
       </c>
     </row>
     <row r="409" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A409" t="s">
+      <c r="A409" s="1" t="s">
         <v>406</v>
       </c>
     </row>
     <row r="410" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A410" t="s">
+      <c r="A410" s="1" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="411" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A411" t="s">
+      <c r="A411" s="1" t="s">
         <v>408</v>
       </c>
     </row>
     <row r="412" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A412" t="s">
+      <c r="A412" s="1" t="s">
         <v>409</v>
       </c>
     </row>
     <row r="413" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A413" t="s">
+      <c r="A413" s="1" t="s">
         <v>410</v>
       </c>
     </row>
     <row r="414" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A414" t="s">
+      <c r="A414" s="1" t="s">
         <v>411</v>
       </c>
     </row>
     <row r="415" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A415" t="s">
+      <c r="A415" s="1" t="s">
         <v>412</v>
       </c>
     </row>
     <row r="416" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A416" t="s">
+      <c r="A416" s="1" t="s">
         <v>413</v>
       </c>
     </row>
     <row r="417" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A417" t="s">
+      <c r="A417" s="1" t="s">
         <v>414</v>
       </c>
     </row>
     <row r="418" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A418" t="s">
+      <c r="A418" s="1" t="s">
         <v>415</v>
       </c>
     </row>
@@ -5008,62 +5009,62 @@
       </c>
     </row>
     <row r="420" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A420" t="s">
+      <c r="A420" s="1" t="s">
         <v>417</v>
       </c>
     </row>
     <row r="421" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A421" t="s">
+      <c r="A421" s="1" t="s">
         <v>418</v>
       </c>
     </row>
     <row r="422" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A422" t="s">
+      <c r="A422" s="1" t="s">
         <v>419</v>
       </c>
     </row>
     <row r="423" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A423" t="s">
+      <c r="A423" s="1" t="s">
         <v>420</v>
       </c>
     </row>
     <row r="424" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A424" t="s">
+      <c r="A424" s="1" t="s">
         <v>421</v>
       </c>
     </row>
     <row r="425" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A425" t="s">
+      <c r="A425" s="1" t="s">
         <v>422</v>
       </c>
     </row>
     <row r="426" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A426" t="s">
+      <c r="A426" s="1" t="s">
         <v>423</v>
       </c>
     </row>
     <row r="427" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A427" t="s">
+      <c r="A427" s="1" t="s">
         <v>424</v>
       </c>
     </row>
     <row r="428" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A428" t="s">
+      <c r="A428" s="1" t="s">
         <v>425</v>
       </c>
     </row>
     <row r="429" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A429" t="s">
+      <c r="A429" s="1" t="s">
         <v>426</v>
       </c>
     </row>
     <row r="430" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A430" t="s">
+      <c r="A430" s="1" t="s">
         <v>427</v>
       </c>
     </row>
     <row r="431" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A431" t="s">
+      <c r="A431" s="1" t="s">
         <v>428</v>
       </c>
     </row>
@@ -5073,7 +5074,7 @@
       </c>
     </row>
     <row r="433" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A433" t="s">
+      <c r="A433" s="1" t="s">
         <v>430</v>
       </c>
     </row>
@@ -5083,57 +5084,57 @@
       </c>
     </row>
     <row r="435" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A435" t="s">
+      <c r="A435" s="1" t="s">
         <v>432</v>
       </c>
     </row>
     <row r="436" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A436" t="s">
+      <c r="A436" s="1" t="s">
         <v>433</v>
       </c>
     </row>
     <row r="437" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A437" t="s">
+      <c r="A437" s="1" t="s">
         <v>434</v>
       </c>
     </row>
     <row r="438" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A438" t="s">
+      <c r="A438" s="1" t="s">
         <v>435</v>
       </c>
     </row>
     <row r="439" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A439" t="s">
+      <c r="A439" s="1" t="s">
         <v>436</v>
       </c>
     </row>
     <row r="440" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A440" t="s">
+      <c r="A440" s="1" t="s">
         <v>437</v>
       </c>
     </row>
     <row r="441" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A441" t="s">
+      <c r="A441" s="1" t="s">
         <v>438</v>
       </c>
     </row>
     <row r="442" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A442" t="s">
+      <c r="A442" s="1" t="s">
         <v>439</v>
       </c>
     </row>
     <row r="443" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A443" t="s">
+      <c r="A443" s="1" t="s">
         <v>440</v>
       </c>
     </row>
     <row r="444" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A444" t="s">
+      <c r="A444" s="1" t="s">
         <v>441</v>
       </c>
     </row>
     <row r="445" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A445" t="s">
+      <c r="A445" s="1" t="s">
         <v>442</v>
       </c>
     </row>
@@ -5143,7 +5144,7 @@
       </c>
     </row>
     <row r="447" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A447" t="s">
+      <c r="A447" s="1" t="s">
         <v>444</v>
       </c>
     </row>
@@ -5153,27 +5154,27 @@
       </c>
     </row>
     <row r="449" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A449" t="s">
+      <c r="A449" s="1" t="s">
         <v>446</v>
       </c>
     </row>
     <row r="450" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A450" t="s">
+      <c r="A450" s="1" t="s">
         <v>447</v>
       </c>
     </row>
     <row r="451" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A451" t="s">
+      <c r="A451" s="1" t="s">
         <v>448</v>
       </c>
     </row>
     <row r="452" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A452" t="s">
+      <c r="A452" s="1" t="s">
         <v>449</v>
       </c>
     </row>
     <row r="453" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A453" t="s">
+      <c r="A453" s="1" t="s">
         <v>450</v>
       </c>
     </row>
@@ -5183,97 +5184,97 @@
       </c>
     </row>
     <row r="455" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A455" t="s">
+      <c r="A455" s="1" t="s">
         <v>452</v>
       </c>
     </row>
     <row r="456" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A456" t="s">
+      <c r="A456" s="1" t="s">
         <v>453</v>
       </c>
     </row>
     <row r="457" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A457" t="s">
+      <c r="A457" s="1" t="s">
         <v>454</v>
       </c>
     </row>
     <row r="458" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A458" t="s">
+      <c r="A458" s="1" t="s">
         <v>455</v>
       </c>
     </row>
     <row r="459" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A459" t="s">
+      <c r="A459" s="1" t="s">
         <v>456</v>
       </c>
     </row>
     <row r="460" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A460" t="s">
+      <c r="A460" s="1" t="s">
         <v>457</v>
       </c>
     </row>
     <row r="461" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A461" t="s">
+      <c r="A461" s="1" t="s">
         <v>458</v>
       </c>
     </row>
     <row r="462" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A462" t="s">
+      <c r="A462" s="1" t="s">
         <v>459</v>
       </c>
     </row>
     <row r="463" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A463" t="s">
+      <c r="A463" s="1" t="s">
         <v>460</v>
       </c>
     </row>
     <row r="464" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A464" t="s">
+      <c r="A464" s="1" t="s">
         <v>461</v>
       </c>
     </row>
     <row r="465" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A465" t="s">
+      <c r="A465" s="1" t="s">
         <v>462</v>
       </c>
     </row>
     <row r="466" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A466" t="s">
+      <c r="A466" s="1" t="s">
         <v>463</v>
       </c>
     </row>
     <row r="467" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A467" t="s">
+      <c r="A467" s="1" t="s">
         <v>464</v>
       </c>
     </row>
     <row r="468" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A468" t="s">
+      <c r="A468" s="1" t="s">
         <v>465</v>
       </c>
     </row>
     <row r="469" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A469" t="s">
+      <c r="A469" s="1" t="s">
         <v>466</v>
       </c>
     </row>
     <row r="470" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A470" t="s">
+      <c r="A470" s="1" t="s">
         <v>467</v>
       </c>
     </row>
     <row r="471" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A471" t="s">
+      <c r="A471" s="1" t="s">
         <v>468</v>
       </c>
     </row>
     <row r="472" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A472" t="s">
+      <c r="A472" s="1" t="s">
         <v>469</v>
       </c>
     </row>
     <row r="473" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A473" t="s">
+      <c r="A473" s="1" t="s">
         <v>186</v>
       </c>
     </row>
@@ -5283,7 +5284,7 @@
       </c>
     </row>
     <row r="475" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A475" t="s">
+      <c r="A475" s="1" t="s">
         <v>471</v>
       </c>
     </row>
@@ -5293,7 +5294,7 @@
       </c>
     </row>
     <row r="477" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A477" t="s">
+      <c r="A477" s="1" t="s">
         <v>473</v>
       </c>
     </row>
@@ -5303,42 +5304,42 @@
       </c>
     </row>
     <row r="479" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A479" t="s">
+      <c r="A479" s="1" t="s">
         <v>475</v>
       </c>
     </row>
     <row r="480" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A480" t="s">
+      <c r="A480" s="1" t="s">
         <v>476</v>
       </c>
     </row>
     <row r="481" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A481" t="s">
+      <c r="A481" s="1" t="s">
         <v>477</v>
       </c>
     </row>
     <row r="482" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A482" t="s">
+      <c r="A482" s="1" t="s">
         <v>478</v>
       </c>
     </row>
     <row r="483" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A483" t="s">
+      <c r="A483" s="1" t="s">
         <v>479</v>
       </c>
     </row>
     <row r="484" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A484" t="s">
+      <c r="A484" s="1" t="s">
         <v>480</v>
       </c>
     </row>
     <row r="485" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A485" t="s">
+      <c r="A485" s="1" t="s">
         <v>481</v>
       </c>
     </row>
     <row r="486" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A486" t="s">
+      <c r="A486" s="1" t="s">
         <v>482</v>
       </c>
     </row>
@@ -5348,188 +5349,188 @@
       </c>
     </row>
     <row r="488" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A488" t="s">
+      <c r="A488" s="1" t="s">
         <v>484</v>
       </c>
     </row>
     <row r="489" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A489" t="s">
+      <c r="A489" s="1" t="s">
         <v>485</v>
       </c>
     </row>
     <row r="490" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A490" t="s">
+      <c r="A490" s="1" t="s">
         <v>486</v>
       </c>
     </row>
     <row r="491" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A491" t="s">
+      <c r="A491" s="1" t="s">
         <v>487</v>
       </c>
     </row>
     <row r="492" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A492" t="s">
+      <c r="A492" s="1" t="s">
         <v>488</v>
       </c>
     </row>
     <row r="493" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A493" t="s">
+      <c r="A493" s="1" t="s">
         <v>489</v>
       </c>
     </row>
     <row r="494" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A494" t="s">
+      <c r="A494" s="1" t="s">
         <v>490</v>
       </c>
     </row>
     <row r="495" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A495" t="s">
+      <c r="A495" s="1" t="s">
         <v>491</v>
       </c>
     </row>
     <row r="496" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A496" t="s">
+      <c r="A496" s="1" t="s">
         <v>492</v>
       </c>
     </row>
     <row r="497" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A497" t="e" cm="1">
+      <c r="A497" s="1" t="e" cm="1">
         <f t="array" ref="A497">-dije yo entre mí.</f>
         <v>#NAME?</v>
       </c>
     </row>
     <row r="498" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A498" t="s">
+      <c r="A498" s="1" t="s">
         <v>493</v>
       </c>
     </row>
     <row r="499" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A499" t="s">
+      <c r="A499" s="1" t="s">
         <v>494</v>
       </c>
     </row>
     <row r="500" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A500" t="s">
+      <c r="A500" s="1" t="s">
         <v>495</v>
       </c>
     </row>
     <row r="501" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A501" t="s">
+      <c r="A501" s="1" t="s">
         <v>496</v>
       </c>
     </row>
     <row r="502" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A502" t="s">
+      <c r="A502" s="1" t="s">
         <v>497</v>
       </c>
     </row>
     <row r="503" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A503" t="s">
+      <c r="A503" s="1" t="s">
         <v>498</v>
       </c>
     </row>
     <row r="504" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A504" t="s">
+      <c r="A504" s="1" t="s">
         <v>499</v>
       </c>
     </row>
     <row r="505" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A505" t="s">
+      <c r="A505" s="1" t="s">
         <v>500</v>
       </c>
     </row>
     <row r="506" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A506" t="s">
+      <c r="A506" s="1" t="s">
         <v>501</v>
       </c>
     </row>
     <row r="507" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A507" t="s">
+      <c r="A507" s="1" t="s">
         <v>502</v>
       </c>
     </row>
     <row r="508" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A508" t="s">
+      <c r="A508" s="1" t="s">
         <v>503</v>
       </c>
     </row>
     <row r="509" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A509" t="s">
+      <c r="A509" s="1" t="s">
         <v>504</v>
       </c>
     </row>
     <row r="510" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A510" t="s">
+      <c r="A510" s="1" t="s">
         <v>505</v>
       </c>
     </row>
     <row r="511" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A511" t="s">
+      <c r="A511" s="1" t="s">
         <v>506</v>
       </c>
     </row>
     <row r="512" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A512" t="s">
+      <c r="A512" s="1" t="s">
         <v>507</v>
       </c>
     </row>
     <row r="513" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A513" t="s">
+      <c r="A513" s="1" t="s">
         <v>508</v>
       </c>
     </row>
     <row r="514" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A514" t="s">
+      <c r="A514" s="1" t="s">
         <v>509</v>
       </c>
     </row>
     <row r="515" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A515" t="s">
+      <c r="A515" s="1" t="s">
         <v>510</v>
       </c>
     </row>
     <row r="516" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A516" t="s">
+      <c r="A516" s="1" t="s">
         <v>511</v>
       </c>
     </row>
     <row r="517" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A517" t="s">
+      <c r="A517" s="1" t="s">
         <v>512</v>
       </c>
     </row>
     <row r="518" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A518" t="s">
+      <c r="A518" s="1" t="s">
         <v>513</v>
       </c>
     </row>
     <row r="519" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A519" t="s">
+      <c r="A519" s="1" t="s">
         <v>514</v>
       </c>
     </row>
     <row r="520" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A520" t="s">
+      <c r="A520" s="1" t="s">
         <v>515</v>
       </c>
     </row>
     <row r="521" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A521" t="s">
+      <c r="A521" s="1" t="s">
         <v>516</v>
       </c>
     </row>
     <row r="522" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A522" t="s">
+      <c r="A522" s="1" t="s">
         <v>517</v>
       </c>
     </row>
     <row r="523" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A523" t="s">
+      <c r="A523" s="1" t="s">
         <v>518</v>
       </c>
     </row>
     <row r="524" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A524" t="s">
+      <c r="A524" s="1" t="s">
         <v>519</v>
       </c>
     </row>
@@ -5539,12 +5540,12 @@
       </c>
     </row>
     <row r="526" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A526" t="s">
+      <c r="A526" s="1" t="s">
         <v>521</v>
       </c>
     </row>
     <row r="527" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A527" t="s">
+      <c r="A527" s="1" t="s">
         <v>522</v>
       </c>
     </row>
@@ -5554,27 +5555,27 @@
       </c>
     </row>
     <row r="529" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A529" t="s">
+      <c r="A529" s="1" t="s">
         <v>524</v>
       </c>
     </row>
     <row r="530" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A530" t="s">
+      <c r="A530" s="1" t="s">
         <v>525</v>
       </c>
     </row>
     <row r="531" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A531" t="s">
+      <c r="A531" s="1" t="s">
         <v>526</v>
       </c>
     </row>
     <row r="532" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A532" t="s">
+      <c r="A532" s="1" t="s">
         <v>527</v>
       </c>
     </row>
     <row r="533" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A533" t="s">
+      <c r="A533" s="1" t="s">
         <v>528</v>
       </c>
     </row>
@@ -5584,7 +5585,7 @@
       </c>
     </row>
     <row r="535" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A535" t="s">
+      <c r="A535" s="1" t="s">
         <v>530</v>
       </c>
     </row>
@@ -5594,17 +5595,17 @@
       </c>
     </row>
     <row r="537" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A537" t="s">
+      <c r="A537" s="1" t="s">
         <v>532</v>
       </c>
     </row>
     <row r="538" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A538" t="s">
+      <c r="A538" s="1" t="s">
         <v>533</v>
       </c>
     </row>
     <row r="539" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A539" t="s">
+      <c r="A539" s="1" t="s">
         <v>534</v>
       </c>
     </row>
@@ -5614,7 +5615,7 @@
       </c>
     </row>
     <row r="541" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A541" t="s">
+      <c r="A541" s="1" t="s">
         <v>536</v>
       </c>
     </row>
@@ -5629,82 +5630,82 @@
       </c>
     </row>
     <row r="544" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A544" t="s">
+      <c r="A544" s="1" t="s">
         <v>539</v>
       </c>
     </row>
     <row r="545" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A545" t="s">
+      <c r="A545" s="1" t="s">
         <v>540</v>
       </c>
     </row>
     <row r="546" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A546" t="s">
+      <c r="A546" s="1" t="s">
         <v>541</v>
       </c>
     </row>
     <row r="547" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A547" t="s">
+      <c r="A547" s="1" t="s">
         <v>542</v>
       </c>
     </row>
     <row r="548" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A548" t="s">
+      <c r="A548" s="1" t="s">
         <v>543</v>
       </c>
     </row>
     <row r="549" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A549" t="s">
+      <c r="A549" s="1" t="s">
         <v>544</v>
       </c>
     </row>
     <row r="550" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A550" t="s">
+      <c r="A550" s="1" t="s">
         <v>545</v>
       </c>
     </row>
     <row r="551" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A551" t="s">
+      <c r="A551" s="1" t="s">
         <v>546</v>
       </c>
     </row>
     <row r="552" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A552" t="s">
+      <c r="A552" s="1" t="s">
         <v>547</v>
       </c>
     </row>
     <row r="553" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A553" t="s">
+      <c r="A553" s="1" t="s">
         <v>548</v>
       </c>
     </row>
     <row r="554" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A554" t="s">
+      <c r="A554" s="1" t="s">
         <v>549</v>
       </c>
     </row>
     <row r="555" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A555" t="s">
+      <c r="A555" s="1" t="s">
         <v>550</v>
       </c>
     </row>
     <row r="556" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A556" t="s">
+      <c r="A556" s="1" t="s">
         <v>551</v>
       </c>
     </row>
     <row r="557" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A557" t="s">
+      <c r="A557" s="1" t="s">
         <v>552</v>
       </c>
     </row>
     <row r="558" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A558" t="s">
+      <c r="A558" s="1" t="s">
         <v>553</v>
       </c>
     </row>
     <row r="559" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A559" t="s">
+      <c r="A559" s="1" t="s">
         <v>554</v>
       </c>
     </row>
@@ -5714,7 +5715,7 @@
       </c>
     </row>
     <row r="561" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A561" t="s">
+      <c r="A561" s="1" t="s">
         <v>556</v>
       </c>
     </row>
@@ -5724,7 +5725,7 @@
       </c>
     </row>
     <row r="563" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A563" t="s">
+      <c r="A563" s="1" t="s">
         <v>558</v>
       </c>
     </row>
@@ -5734,97 +5735,97 @@
       </c>
     </row>
     <row r="565" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A565" t="s">
+      <c r="A565" s="1" t="s">
         <v>560</v>
       </c>
     </row>
     <row r="566" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A566" t="s">
+      <c r="A566" s="1" t="s">
         <v>561</v>
       </c>
     </row>
     <row r="567" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A567" t="s">
+      <c r="A567" s="1" t="s">
         <v>562</v>
       </c>
     </row>
     <row r="568" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A568" t="s">
+      <c r="A568" s="1" t="s">
         <v>563</v>
       </c>
     </row>
     <row r="569" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A569" t="s">
+      <c r="A569" s="1" t="s">
         <v>564</v>
       </c>
     </row>
     <row r="570" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A570" t="s">
+      <c r="A570" s="1" t="s">
         <v>565</v>
       </c>
     </row>
     <row r="571" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A571" t="s">
+      <c r="A571" s="1" t="s">
         <v>566</v>
       </c>
     </row>
     <row r="572" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A572" t="s">
+      <c r="A572" s="1" t="s">
         <v>567</v>
       </c>
     </row>
     <row r="573" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A573" t="s">
+      <c r="A573" s="1" t="s">
         <v>568</v>
       </c>
     </row>
     <row r="574" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A574" t="s">
+      <c r="A574" s="1" t="s">
         <v>569</v>
       </c>
     </row>
     <row r="575" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A575" t="s">
+      <c r="A575" s="1" t="s">
         <v>570</v>
       </c>
     </row>
     <row r="576" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A576" t="s">
+      <c r="A576" s="1" t="s">
         <v>571</v>
       </c>
     </row>
     <row r="577" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A577" t="s">
+      <c r="A577" s="1" t="s">
         <v>572</v>
       </c>
     </row>
     <row r="578" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A578" t="s">
+      <c r="A578" s="1" t="s">
         <v>573</v>
       </c>
     </row>
     <row r="579" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A579" t="s">
+      <c r="A579" s="1" t="s">
         <v>574</v>
       </c>
     </row>
     <row r="580" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A580" t="s">
+      <c r="A580" s="1" t="s">
         <v>575</v>
       </c>
     </row>
     <row r="581" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A581" t="s">
+      <c r="A581" s="1" t="s">
         <v>576</v>
       </c>
     </row>
     <row r="582" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A582" t="s">
+      <c r="A582" s="1" t="s">
         <v>577</v>
       </c>
     </row>
     <row r="583" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A583" t="s">
+      <c r="A583" s="1" t="s">
         <v>578</v>
       </c>
     </row>
@@ -5834,32 +5835,32 @@
       </c>
     </row>
     <row r="585" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A585" t="s">
+      <c r="A585" s="1" t="s">
         <v>580</v>
       </c>
     </row>
     <row r="586" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A586" t="s">
+      <c r="A586" s="1" t="s">
         <v>581</v>
       </c>
     </row>
     <row r="587" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A587" t="s">
+      <c r="A587" s="1" t="s">
         <v>582</v>
       </c>
     </row>
     <row r="588" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A588" t="s">
+      <c r="A588" s="1" t="s">
         <v>583</v>
       </c>
     </row>
     <row r="589" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A589" t="s">
+      <c r="A589" s="1" t="s">
         <v>584</v>
       </c>
     </row>
     <row r="590" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A590" t="s">
+      <c r="A590" s="1" t="s">
         <v>585</v>
       </c>
     </row>
@@ -5869,7 +5870,7 @@
       </c>
     </row>
     <row r="592" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A592" t="s">
+      <c r="A592" s="1" t="s">
         <v>587</v>
       </c>
     </row>
@@ -5879,267 +5880,267 @@
       </c>
     </row>
     <row r="594" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A594" t="s">
+      <c r="A594" s="1" t="s">
         <v>589</v>
       </c>
     </row>
     <row r="595" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A595" t="s">
+      <c r="A595" s="1" t="s">
         <v>590</v>
       </c>
     </row>
     <row r="596" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A596" t="s">
+      <c r="A596" s="1" t="s">
         <v>591</v>
       </c>
     </row>
     <row r="597" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A597" t="s">
+      <c r="A597" s="1" t="s">
         <v>592</v>
       </c>
     </row>
     <row r="598" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A598" t="s">
+      <c r="A598" s="1" t="s">
         <v>593</v>
       </c>
     </row>
     <row r="599" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A599" t="s">
+      <c r="A599" s="1" t="s">
         <v>594</v>
       </c>
     </row>
     <row r="600" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A600" t="s">
+      <c r="A600" s="1" t="s">
         <v>595</v>
       </c>
     </row>
     <row r="601" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A601" t="s">
+      <c r="A601" s="1" t="s">
         <v>596</v>
       </c>
     </row>
     <row r="602" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A602" t="s">
+      <c r="A602" s="1" t="s">
         <v>597</v>
       </c>
     </row>
     <row r="603" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A603" t="s">
+      <c r="A603" s="1" t="s">
         <v>598</v>
       </c>
     </row>
     <row r="604" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A604" t="s">
+      <c r="A604" s="1" t="s">
         <v>599</v>
       </c>
     </row>
     <row r="605" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A605" t="s">
+      <c r="A605" s="1" t="s">
         <v>600</v>
       </c>
     </row>
     <row r="606" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A606" t="s">
+      <c r="A606" s="1" t="s">
         <v>601</v>
       </c>
     </row>
     <row r="607" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A607" t="s">
+      <c r="A607" s="1" t="s">
         <v>602</v>
       </c>
     </row>
     <row r="608" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A608" t="s">
+      <c r="A608" s="1" t="s">
         <v>603</v>
       </c>
     </row>
     <row r="609" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A609" t="s">
+      <c r="A609" s="1" t="s">
         <v>604</v>
       </c>
     </row>
     <row r="610" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A610" t="s">
+      <c r="A610" s="1" t="s">
         <v>605</v>
       </c>
     </row>
     <row r="611" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A611" t="s">
+      <c r="A611" s="1" t="s">
         <v>606</v>
       </c>
     </row>
     <row r="612" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A612" t="s">
+      <c r="A612" s="1" t="s">
         <v>607</v>
       </c>
     </row>
     <row r="613" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A613" t="s">
+      <c r="A613" s="1" t="s">
         <v>608</v>
       </c>
     </row>
     <row r="614" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A614" t="s">
+      <c r="A614" s="1" t="s">
         <v>609</v>
       </c>
     </row>
     <row r="615" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A615" t="s">
+      <c r="A615" s="1" t="s">
         <v>610</v>
       </c>
     </row>
     <row r="616" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A616" t="s">
+      <c r="A616" s="1" t="s">
         <v>611</v>
       </c>
     </row>
     <row r="617" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A617" t="s">
+      <c r="A617" s="1" t="s">
         <v>612</v>
       </c>
     </row>
     <row r="618" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A618" t="s">
+      <c r="A618" s="1" t="s">
         <v>613</v>
       </c>
     </row>
     <row r="619" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A619" t="s">
+      <c r="A619" s="1" t="s">
         <v>614</v>
       </c>
     </row>
     <row r="620" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A620" t="s">
+      <c r="A620" s="1" t="s">
         <v>615</v>
       </c>
     </row>
     <row r="621" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A621" t="s">
+      <c r="A621" s="1" t="s">
         <v>616</v>
       </c>
     </row>
     <row r="622" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A622" t="s">
+      <c r="A622" s="1" t="s">
         <v>617</v>
       </c>
     </row>
     <row r="623" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A623" t="s">
+      <c r="A623" s="1" t="s">
         <v>618</v>
       </c>
     </row>
     <row r="624" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A624" t="s">
+      <c r="A624" s="1" t="s">
         <v>619</v>
       </c>
     </row>
     <row r="625" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A625" t="s">
+      <c r="A625" s="1" t="s">
         <v>620</v>
       </c>
     </row>
     <row r="626" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A626" t="s">
+      <c r="A626" s="1" t="s">
         <v>621</v>
       </c>
     </row>
     <row r="627" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A627" t="s">
+      <c r="A627" s="1" t="s">
         <v>622</v>
       </c>
     </row>
     <row r="628" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A628" t="s">
+      <c r="A628" s="1" t="s">
         <v>623</v>
       </c>
     </row>
     <row r="629" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A629" t="s">
+      <c r="A629" s="1" t="s">
         <v>624</v>
       </c>
     </row>
     <row r="630" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A630" t="s">
+      <c r="A630" s="1" t="s">
         <v>625</v>
       </c>
     </row>
     <row r="631" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A631" t="s">
+      <c r="A631" s="1" t="s">
         <v>626</v>
       </c>
     </row>
     <row r="632" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A632" t="s">
+      <c r="A632" s="1" t="s">
         <v>627</v>
       </c>
     </row>
     <row r="633" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A633" t="s">
+      <c r="A633" s="1" t="s">
         <v>628</v>
       </c>
     </row>
     <row r="634" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A634" t="s">
+      <c r="A634" s="1" t="s">
         <v>629</v>
       </c>
     </row>
     <row r="635" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A635" t="s">
+      <c r="A635" s="1" t="s">
         <v>630</v>
       </c>
     </row>
     <row r="636" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A636" t="s">
+      <c r="A636" s="1" t="s">
         <v>631</v>
       </c>
     </row>
     <row r="637" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A637" t="s">
+      <c r="A637" s="1" t="s">
         <v>632</v>
       </c>
     </row>
     <row r="638" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A638" t="s">
+      <c r="A638" s="1" t="s">
         <v>633</v>
       </c>
     </row>
     <row r="639" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A639" t="s">
+      <c r="A639" s="1" t="s">
         <v>634</v>
       </c>
     </row>
     <row r="640" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A640" t="s">
+      <c r="A640" s="1" t="s">
         <v>635</v>
       </c>
     </row>
     <row r="641" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A641" t="s">
+      <c r="A641" s="1" t="s">
         <v>636</v>
       </c>
     </row>
     <row r="642" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A642" t="s">
+      <c r="A642" s="1" t="s">
         <v>637</v>
       </c>
     </row>
     <row r="643" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A643" t="s">
+      <c r="A643" s="1" t="s">
         <v>638</v>
       </c>
     </row>
     <row r="644" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A644" t="s">
+      <c r="A644" s="1" t="s">
         <v>639</v>
       </c>
     </row>
     <row r="645" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A645" t="s">
+      <c r="A645" s="1" t="s">
         <v>640</v>
       </c>
     </row>
     <row r="646" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A646" t="s">
+      <c r="A646" s="1" t="s">
         <v>641</v>
       </c>
     </row>
@@ -6149,42 +6150,42 @@
       </c>
     </row>
     <row r="648" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A648" t="s">
+      <c r="A648" s="1" t="s">
         <v>643</v>
       </c>
     </row>
     <row r="649" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A649" t="s">
+      <c r="A649" s="1" t="s">
         <v>644</v>
       </c>
     </row>
     <row r="650" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A650" t="s">
+      <c r="A650" s="1" t="s">
         <v>645</v>
       </c>
     </row>
     <row r="651" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A651" t="s">
+      <c r="A651" s="1" t="s">
         <v>646</v>
       </c>
     </row>
     <row r="652" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A652" t="s">
+      <c r="A652" s="1" t="s">
         <v>647</v>
       </c>
     </row>
     <row r="653" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A653" t="s">
+      <c r="A653" s="1" t="s">
         <v>648</v>
       </c>
     </row>
     <row r="654" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A654" t="s">
+      <c r="A654" s="1" t="s">
         <v>649</v>
       </c>
     </row>
     <row r="655" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A655" t="s">
+      <c r="A655" s="1" t="s">
         <v>650</v>
       </c>
     </row>
@@ -6194,62 +6195,62 @@
       </c>
     </row>
     <row r="657" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A657" t="s">
+      <c r="A657" s="1" t="s">
         <v>652</v>
       </c>
     </row>
     <row r="658" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A658" t="s">
+      <c r="A658" s="1" t="s">
         <v>653</v>
       </c>
     </row>
     <row r="659" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A659" t="s">
+      <c r="A659" s="1" t="s">
         <v>654</v>
       </c>
     </row>
     <row r="660" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A660" t="s">
+      <c r="A660" s="1" t="s">
         <v>655</v>
       </c>
     </row>
     <row r="661" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A661" t="s">
+      <c r="A661" s="1" t="s">
         <v>656</v>
       </c>
     </row>
     <row r="662" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A662" t="s">
+      <c r="A662" s="1" t="s">
         <v>657</v>
       </c>
     </row>
     <row r="663" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A663" t="s">
+      <c r="A663" s="1" t="s">
         <v>658</v>
       </c>
     </row>
     <row r="664" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A664" t="s">
+      <c r="A664" s="1" t="s">
         <v>659</v>
       </c>
     </row>
     <row r="665" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A665" t="s">
+      <c r="A665" s="1" t="s">
         <v>660</v>
       </c>
     </row>
     <row r="666" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A666" t="s">
+      <c r="A666" s="1" t="s">
         <v>661</v>
       </c>
     </row>
     <row r="667" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A667" t="s">
+      <c r="A667" s="1" t="s">
         <v>662</v>
       </c>
     </row>
     <row r="668" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A668" t="s">
+      <c r="A668" s="1" t="s">
         <v>663</v>
       </c>
     </row>
@@ -6259,67 +6260,67 @@
       </c>
     </row>
     <row r="670" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A670" t="s">
+      <c r="A670" s="1" t="s">
         <v>665</v>
       </c>
     </row>
     <row r="671" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A671" t="s">
+      <c r="A671" s="1" t="s">
         <v>666</v>
       </c>
     </row>
     <row r="672" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A672" t="s">
+      <c r="A672" s="1" t="s">
         <v>667</v>
       </c>
     </row>
     <row r="673" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A673" t="s">
+      <c r="A673" s="1" t="s">
         <v>668</v>
       </c>
     </row>
     <row r="674" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A674" t="s">
+      <c r="A674" s="1" t="s">
         <v>669</v>
       </c>
     </row>
     <row r="675" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A675" t="s">
+      <c r="A675" s="1" t="s">
         <v>670</v>
       </c>
     </row>
     <row r="676" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A676" t="s">
+      <c r="A676" s="1" t="s">
         <v>671</v>
       </c>
     </row>
     <row r="677" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A677" t="s">
+      <c r="A677" s="1" t="s">
         <v>672</v>
       </c>
     </row>
     <row r="678" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A678" t="s">
+      <c r="A678" s="1" t="s">
         <v>673</v>
       </c>
     </row>
     <row r="679" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A679" t="s">
+      <c r="A679" s="1" t="s">
         <v>674</v>
       </c>
     </row>
     <row r="680" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A680" t="s">
+      <c r="A680" s="1" t="s">
         <v>675</v>
       </c>
     </row>
     <row r="681" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A681" t="s">
+      <c r="A681" s="1" t="s">
         <v>676</v>
       </c>
     </row>
     <row r="682" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A682" t="s">
+      <c r="A682" s="1" t="s">
         <v>677</v>
       </c>
     </row>
@@ -6329,117 +6330,117 @@
       </c>
     </row>
     <row r="684" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A684" t="s">
+      <c r="A684" s="1" t="s">
         <v>679</v>
       </c>
     </row>
     <row r="685" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A685" t="s">
+      <c r="A685" s="1" t="s">
         <v>680</v>
       </c>
     </row>
     <row r="686" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A686" t="s">
+      <c r="A686" s="1" t="s">
         <v>681</v>
       </c>
     </row>
     <row r="687" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A687" t="s">
+      <c r="A687" s="1" t="s">
         <v>682</v>
       </c>
     </row>
     <row r="688" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A688" t="s">
+      <c r="A688" s="1" t="s">
         <v>683</v>
       </c>
     </row>
     <row r="689" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A689" t="s">
+      <c r="A689" s="1" t="s">
         <v>684</v>
       </c>
     </row>
     <row r="690" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A690" t="s">
+      <c r="A690" s="1" t="s">
         <v>685</v>
       </c>
     </row>
     <row r="691" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A691" t="s">
+      <c r="A691" s="1" t="s">
         <v>686</v>
       </c>
     </row>
     <row r="692" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A692" t="s">
+      <c r="A692" s="1" t="s">
         <v>687</v>
       </c>
     </row>
     <row r="693" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A693" t="s">
+      <c r="A693" s="1" t="s">
         <v>688</v>
       </c>
     </row>
     <row r="694" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A694" t="s">
+      <c r="A694" s="1" t="s">
         <v>689</v>
       </c>
     </row>
     <row r="695" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A695" t="s">
+      <c r="A695" s="1" t="s">
         <v>690</v>
       </c>
     </row>
     <row r="696" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A696" t="s">
+      <c r="A696" s="1" t="s">
         <v>691</v>
       </c>
     </row>
     <row r="697" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A697" t="s">
+      <c r="A697" s="1" t="s">
         <v>692</v>
       </c>
     </row>
     <row r="698" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A698" t="s">
+      <c r="A698" s="1" t="s">
         <v>693</v>
       </c>
     </row>
     <row r="699" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A699" t="s">
+      <c r="A699" s="1" t="s">
         <v>694</v>
       </c>
     </row>
     <row r="700" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A700" t="s">
+      <c r="A700" s="1" t="s">
         <v>695</v>
       </c>
     </row>
     <row r="701" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A701" t="s">
+      <c r="A701" s="1" t="s">
         <v>696</v>
       </c>
     </row>
     <row r="702" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A702" t="s">
+      <c r="A702" s="1" t="s">
         <v>697</v>
       </c>
     </row>
     <row r="703" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A703" t="s">
+      <c r="A703" s="1" t="s">
         <v>698</v>
       </c>
     </row>
     <row r="704" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A704" t="s">
+      <c r="A704" s="1" t="s">
         <v>699</v>
       </c>
     </row>
     <row r="705" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A705" t="s">
+      <c r="A705" s="1" t="s">
         <v>700</v>
       </c>
     </row>
     <row r="706" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A706" t="s">
+      <c r="A706" s="1" t="s">
         <v>701</v>
       </c>
     </row>
@@ -6449,7 +6450,7 @@
       </c>
     </row>
     <row r="708" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A708" t="s">
+      <c r="A708" s="1" t="s">
         <v>703</v>
       </c>
     </row>
@@ -6459,287 +6460,287 @@
       </c>
     </row>
     <row r="710" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A710" t="s">
+      <c r="A710" s="1" t="s">
         <v>705</v>
       </c>
     </row>
     <row r="711" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A711" t="s">
+      <c r="A711" s="1" t="s">
         <v>706</v>
       </c>
     </row>
     <row r="712" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A712" t="s">
+      <c r="A712" s="1" t="s">
         <v>707</v>
       </c>
     </row>
     <row r="713" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A713" t="s">
+      <c r="A713" s="1" t="s">
         <v>708</v>
       </c>
     </row>
     <row r="714" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A714" t="s">
+      <c r="A714" s="1" t="s">
         <v>709</v>
       </c>
     </row>
     <row r="715" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A715" t="s">
+      <c r="A715" s="1" t="s">
         <v>710</v>
       </c>
     </row>
     <row r="716" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A716" t="s">
+      <c r="A716" s="1" t="s">
         <v>711</v>
       </c>
     </row>
     <row r="717" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A717" t="s">
+      <c r="A717" s="1" t="s">
         <v>712</v>
       </c>
     </row>
     <row r="718" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A718" t="s">
+      <c r="A718" s="1" t="s">
         <v>713</v>
       </c>
     </row>
     <row r="719" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A719" t="s">
+      <c r="A719" s="1" t="s">
         <v>714</v>
       </c>
     </row>
     <row r="720" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A720" t="s">
+      <c r="A720" s="1" t="s">
         <v>715</v>
       </c>
     </row>
     <row r="721" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A721" t="s">
+      <c r="A721" s="1" t="s">
         <v>716</v>
       </c>
     </row>
     <row r="722" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A722" t="s">
+      <c r="A722" s="1" t="s">
         <v>717</v>
       </c>
     </row>
     <row r="723" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A723" t="s">
+      <c r="A723" s="1" t="s">
         <v>718</v>
       </c>
     </row>
     <row r="724" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A724" t="s">
+      <c r="A724" s="1" t="s">
         <v>719</v>
       </c>
     </row>
     <row r="725" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A725" t="s">
+      <c r="A725" s="1" t="s">
         <v>720</v>
       </c>
     </row>
     <row r="726" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A726" t="s">
+      <c r="A726" s="1" t="s">
         <v>721</v>
       </c>
     </row>
     <row r="727" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A727" t="s">
+      <c r="A727" s="1" t="s">
         <v>722</v>
       </c>
     </row>
     <row r="728" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A728" t="s">
+      <c r="A728" s="1" t="s">
         <v>723</v>
       </c>
     </row>
     <row r="729" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A729" t="s">
+      <c r="A729" s="1" t="s">
         <v>724</v>
       </c>
     </row>
     <row r="730" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A730" t="s">
+      <c r="A730" s="1" t="s">
         <v>725</v>
       </c>
     </row>
     <row r="731" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A731" t="s">
+      <c r="A731" s="1" t="s">
         <v>726</v>
       </c>
     </row>
     <row r="732" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A732" t="s">
+      <c r="A732" s="1" t="s">
         <v>727</v>
       </c>
     </row>
     <row r="733" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A733" t="s">
+      <c r="A733" s="1" t="s">
         <v>728</v>
       </c>
     </row>
     <row r="734" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A734" t="s">
+      <c r="A734" s="1" t="s">
         <v>729</v>
       </c>
     </row>
     <row r="735" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A735" t="s">
+      <c r="A735" s="1" t="s">
         <v>730</v>
       </c>
     </row>
     <row r="736" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A736" t="s">
+      <c r="A736" s="1" t="s">
         <v>731</v>
       </c>
     </row>
     <row r="737" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A737" t="s">
+      <c r="A737" s="1" t="s">
         <v>732</v>
       </c>
     </row>
     <row r="738" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A738" t="s">
+      <c r="A738" s="1" t="s">
         <v>733</v>
       </c>
     </row>
     <row r="739" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A739" t="s">
+      <c r="A739" s="1" t="s">
         <v>734</v>
       </c>
     </row>
     <row r="740" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A740" t="s">
+      <c r="A740" s="1" t="s">
         <v>735</v>
       </c>
     </row>
     <row r="741" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A741" t="s">
+      <c r="A741" s="1" t="s">
         <v>736</v>
       </c>
     </row>
     <row r="742" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A742" t="s">
+      <c r="A742" s="1" t="s">
         <v>737</v>
       </c>
     </row>
     <row r="743" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A743" t="s">
+      <c r="A743" s="1" t="s">
         <v>738</v>
       </c>
     </row>
     <row r="744" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A744" t="s">
+      <c r="A744" s="1" t="s">
         <v>739</v>
       </c>
     </row>
     <row r="745" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A745" t="s">
+      <c r="A745" s="1" t="s">
         <v>740</v>
       </c>
     </row>
     <row r="746" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A746" t="s">
+      <c r="A746" s="1" t="s">
         <v>741</v>
       </c>
     </row>
     <row r="747" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A747" t="s">
+      <c r="A747" s="1" t="s">
         <v>742</v>
       </c>
     </row>
     <row r="748" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A748" t="s">
+      <c r="A748" s="1" t="s">
         <v>743</v>
       </c>
     </row>
     <row r="749" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A749" t="s">
+      <c r="A749" s="1" t="s">
         <v>744</v>
       </c>
     </row>
     <row r="750" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A750" t="s">
+      <c r="A750" s="1" t="s">
         <v>745</v>
       </c>
     </row>
     <row r="751" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A751" t="s">
+      <c r="A751" s="1" t="s">
         <v>746</v>
       </c>
     </row>
     <row r="752" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A752" t="s">
+      <c r="A752" s="1" t="s">
         <v>747</v>
       </c>
     </row>
     <row r="753" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A753" t="s">
+      <c r="A753" s="1" t="s">
         <v>748</v>
       </c>
     </row>
     <row r="754" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A754" t="s">
+      <c r="A754" s="1" t="s">
         <v>749</v>
       </c>
     </row>
     <row r="755" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A755" t="s">
+      <c r="A755" s="1" t="s">
         <v>750</v>
       </c>
     </row>
     <row r="756" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A756" t="s">
+      <c r="A756" s="1" t="s">
         <v>751</v>
       </c>
     </row>
     <row r="757" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A757" t="s">
+      <c r="A757" s="1" t="s">
         <v>752</v>
       </c>
     </row>
     <row r="758" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A758" t="s">
+      <c r="A758" s="1" t="s">
         <v>753</v>
       </c>
     </row>
     <row r="759" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A759" t="s">
+      <c r="A759" s="1" t="s">
         <v>754</v>
       </c>
     </row>
     <row r="760" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A760" t="s">
+      <c r="A760" s="1" t="s">
         <v>755</v>
       </c>
     </row>
     <row r="761" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A761" t="s">
+      <c r="A761" s="1" t="s">
         <v>756</v>
       </c>
     </row>
     <row r="762" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A762" t="s">
+      <c r="A762" s="1" t="s">
         <v>757</v>
       </c>
     </row>
     <row r="763" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A763" t="s">
+      <c r="A763" s="1" t="s">
         <v>758</v>
       </c>
     </row>
     <row r="764" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A764" t="s">
+      <c r="A764" s="1" t="s">
         <v>759</v>
       </c>
     </row>
     <row r="765" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A765" t="s">
+      <c r="A765" s="1" t="s">
         <v>760</v>
       </c>
     </row>
     <row r="766" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A766" t="s">
+      <c r="A766" s="1" t="s">
         <v>761</v>
       </c>
     </row>
@@ -6754,32 +6755,32 @@
       </c>
     </row>
     <row r="769" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A769" t="s">
+      <c r="A769" s="1" t="s">
         <v>764</v>
       </c>
     </row>
     <row r="770" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A770" t="s">
+      <c r="A770" s="1" t="s">
         <v>765</v>
       </c>
     </row>
     <row r="771" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A771" t="s">
+      <c r="A771" s="1" t="s">
         <v>766</v>
       </c>
     </row>
     <row r="772" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A772" t="s">
+      <c r="A772" s="1" t="s">
         <v>767</v>
       </c>
     </row>
     <row r="773" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A773" t="s">
+      <c r="A773" s="1" t="s">
         <v>768</v>
       </c>
     </row>
     <row r="774" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A774" t="s">
+      <c r="A774" s="1" t="s">
         <v>769</v>
       </c>
     </row>
@@ -6789,27 +6790,27 @@
       </c>
     </row>
     <row r="776" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A776" t="s">
+      <c r="A776" s="1" t="s">
         <v>771</v>
       </c>
     </row>
     <row r="777" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A777" t="s">
+      <c r="A777" s="1" t="s">
         <v>772</v>
       </c>
     </row>
     <row r="778" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A778" t="s">
+      <c r="A778" s="1" t="s">
         <v>773</v>
       </c>
     </row>
     <row r="779" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A779" t="s">
+      <c r="A779" s="1" t="s">
         <v>774</v>
       </c>
     </row>
     <row r="780" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A780" t="s">
+      <c r="A780" s="1" t="s">
         <v>775</v>
       </c>
     </row>

</xml_diff>